<commit_message>
feat(TTrack): Concludes new Engine Matching updates (Closes #51)
</commit_message>
<xml_diff>
--- a/T1-SDM/projects/TTrack_v1/services/data/sample_academic_transcript_v2.xlsx
+++ b/T1-SDM/projects/TTrack_v1/services/data/sample_academic_transcript_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luisfaria/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB44DB77-9E42-AD49-B6B0-47F3FDDA9427}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8BFA02D-74C8-0648-89E5-1D130655609F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="21060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="28">
   <si>
     <t>Year</t>
   </si>
@@ -105,6 +105,18 @@
   </si>
   <si>
     <t>Student A</t>
+  </si>
+  <si>
+    <t>Course Name</t>
+  </si>
+  <si>
+    <t>Student ID</t>
+  </si>
+  <si>
+    <t>Associate Degree of Information Technology</t>
+  </si>
+  <si>
+    <t>A00123456</t>
   </si>
 </sst>
 </file>
@@ -382,16 +394,18 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="4" max="4" width="27.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -416,8 +430,14 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1">
         <v>2023</v>
       </c>
@@ -442,8 +462,14 @@
       <c r="H2" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="I2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1">
         <v>2023</v>
       </c>
@@ -468,8 +494,14 @@
       <c r="H3" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="I3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1">
         <v>2024</v>
       </c>
@@ -494,8 +526,14 @@
       <c r="H4" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="I4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1">
         <v>2024</v>
       </c>
@@ -520,8 +558,14 @@
       <c r="H5" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="I5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1">
         <v>2025</v>
       </c>
@@ -546,8 +590,14 @@
       <c r="H6" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="I6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1">
         <v>2025</v>
       </c>
@@ -571,6 +621,12 @@
       </c>
       <c r="H7" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>